<commit_message>
get -> get_check 변경
</commit_message>
<xml_diff>
--- a/Plan/Data_추출파일/008.티니핑도감테이블.xlsx
+++ b/Plan/Data_추출파일/008.티니핑도감테이블.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Solid8\Desktop\Tiniffing_plan\Plan\Data_추출파일\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{17649028-EBDA-4A31-B474-FD15CDC33566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A4FADA3E-9EE3-4B33-B17B-74ADD2758225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A66F5B9B-CCD0-4CFA-AB14-197AE1C1E0EA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C36C76D9-08C1-4DF5-A4A7-A05734BE4FAD}"/>
   </bookViews>
   <sheets>
     <sheet name="008.티니핑도감테이블" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
     <t>tiniffing_name</t>
   </si>
   <si>
-    <t>get</t>
+    <t>get_check</t>
   </si>
   <si>
     <t>name_text_id</t>
@@ -411,7 +411,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{869E8002-F615-4F7A-ABF9-770DE97180F5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B41F704-C572-4B05-AEA6-5FE8F45FD7A6}">
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">

</xml_diff>